<commit_message>
Two players working version with soooo many bugs and needs enhancements
</commit_message>
<xml_diff>
--- a/python/players.xlsx
+++ b/python/players.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/t0b090k/PycharmProjects/workarea/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/t0b090k/StudioProjects/CricketCards/python/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80CB824E-565A-DB4D-8A38-8728AF7DAB9D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{214239B3-F757-AC4E-A029-4184708D4E79}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16180" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16180" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="bengaluru" sheetId="1" r:id="rId1"/>
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2969" uniqueCount="1524">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2969" uniqueCount="1523">
   <si>
     <t>id</t>
   </si>
@@ -4617,9 +4617,6 @@
   </si>
   <si>
     <t>3/18)</t>
-  </si>
-  <si>
-    <t>Id</t>
   </si>
 </sst>
 </file>
@@ -5023,7 +5020,7 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:Z23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="Y24" sqref="Y24"/>
     </sheetView>
   </sheetViews>
@@ -6460,7 +6457,7 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:Z26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
@@ -6472,7 +6469,7 @@
   <sheetData>
     <row r="1" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>1523</v>
+        <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>

</xml_diff>